<commit_message>
Updated Config and Readme
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\bands_bookings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC4494A7-3E13-4FC8-A1DC-16D5E97296B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE27547-C57F-435B-8839-DF9AAF97A62E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Name</t>
   </si>
@@ -81,13 +81,41 @@
   </si>
   <si>
     <t>chengxin_lee@mymail.sutd.edu.sg</t>
+  </si>
+  <si>
+    <r>
+      <t>D:\bookings\</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF191970"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>booking-venv</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>\Scripts\activate.ps1</t>
+    </r>
+  </si>
+  <si>
+    <t>Path to .pst activate script for venv</t>
+  </si>
+  <si>
+    <t>venv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -115,6 +143,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF191970"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -462,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -539,6 +573,17 @@
         <v>14</v>
       </c>
     </row>
+    <row r="7" spans="1:3" ht="15" customHeight="1">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>

</xml_diff>